<commit_message>
pscyhoeducation plot updated to new scale
</commit_message>
<xml_diff>
--- a/data/suma_psychoeducation.xlsx
+++ b/data/suma_psychoeducation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/Dissertation/Pilot Data/summer_pilot/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52671184-47B1-A840-ACB6-CE9D74D89C46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABA321B-DCCD-3C46-825A-A42D0FE1A03F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35200" yWindow="5020" windowWidth="27240" windowHeight="15260" xr2:uid="{8F5799AF-0C4B-0F45-9DEC-58DC67562516}"/>
+    <workbookView xWindow="33420" yWindow="5040" windowWidth="27240" windowHeight="15260" xr2:uid="{8F5799AF-0C4B-0F45-9DEC-58DC67562516}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,12 +33,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>session</t>
   </si>
   <si>
-    <t>pe</t>
+    <t>pe_cl</t>
+  </si>
+  <si>
+    <t>pe_jim</t>
   </si>
 </sst>
 </file>
@@ -390,44 +393,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5C2C51E-D632-F24E-9B03-89BF5A24192A}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>